<commit_message>
Fixed import data Kelola Mahasiswa
</commit_message>
<xml_diff>
--- a/public/Template_Mahasiswa.xlsx
+++ b/public/Template_Mahasiswa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\sipresma\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2B8DA53-A9B1-4C0E-8287-42685A901DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65D7CED-DD49-4C67-8CB8-339E7911CBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4716" yWindow="1764" windowWidth="17280" windowHeight="8880" xr2:uid="{31ED9745-3A25-4EE4-AFCC-90DE7B4ECB14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{31ED9745-3A25-4EE4-AFCC-90DE7B4ECB14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>NIM</t>
   </si>
@@ -100,6 +100,15 @@
   </si>
   <si>
     <t>Jl. Example 5</t>
+  </si>
+  <si>
+    <t>Jenis Kelamin</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -482,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E4BBE4-C093-46EE-AA14-7B59D7F609C4}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="H3" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -496,9 +505,10 @@
     <col min="4" max="4" width="29.109375" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -517,8 +527,11 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2341720111</v>
       </c>
@@ -537,8 +550,11 @@
       <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2341720222</v>
       </c>
@@ -557,8 +573,11 @@
       <c r="F3" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2341720333</v>
       </c>
@@ -577,8 +596,11 @@
       <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2341720444</v>
       </c>
@@ -597,8 +619,11 @@
       <c r="F5" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="G5" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2341720555</v>
       </c>
@@ -616,6 +641,9 @@
       </c>
       <c r="F6" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update status Pendaftaran Lomba (Mahasiswa)
</commit_message>
<xml_diff>
--- a/public/Template_Mahasiswa.xlsx
+++ b/public/Template_Mahasiswa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\sipresma\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65D7CED-DD49-4C67-8CB8-339E7911CBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D32163-8CC0-4FAA-8F6F-7BE3C8DDC7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{31ED9745-3A25-4EE4-AFCC-90DE7B4ECB14}"/>
+    <workbookView xWindow="3912" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{31ED9745-3A25-4EE4-AFCC-90DE7B4ECB14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>NIM</t>
   </si>
@@ -109,6 +109,24 @@
   </si>
   <si>
     <t>P</t>
+  </si>
+  <si>
+    <t>Bidang Minat &amp; Bakat</t>
+  </si>
+  <si>
+    <t>Memancing</t>
+  </si>
+  <si>
+    <t>Mendaki</t>
+  </si>
+  <si>
+    <t>Motoran</t>
+  </si>
+  <si>
+    <t>Membaca</t>
+  </si>
+  <si>
+    <t>Merakit bom</t>
   </si>
 </sst>
 </file>
@@ -491,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E4BBE4-C093-46EE-AA14-7B59D7F609C4}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -506,9 +524,10 @@
     <col min="5" max="5" width="19.6640625" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -530,8 +549,11 @@
       <c r="G1" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2341720111</v>
       </c>
@@ -553,8 +575,11 @@
       <c r="G2" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2341720222</v>
       </c>
@@ -576,8 +601,11 @@
       <c r="G3" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2341720333</v>
       </c>
@@ -599,8 +627,11 @@
       <c r="G4" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="H4" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2341720444</v>
       </c>
@@ -622,8 +653,11 @@
       <c r="G5" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="H5" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2341720555</v>
       </c>
@@ -644,6 +678,9 @@
       </c>
       <c r="G6" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>